<commit_message>
Remove quote number text file logic, patch parallel safety, and update batch/test runner scripts
</commit_message>
<xml_diff>
--- a/WB_Test_Report_2025-12-26.xlsx
+++ b/WB_Test_Report_2025-12-26.xlsx
@@ -4,8 +4,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Package_1" sheetId="2" r:id="rId2"/>
-    <sheet name="Package_2" sheetId="3" r:id="rId3"/>
+    <sheet name="BOP_1" sheetId="2" r:id="rId2"/>
+    <sheet name="BOP_2" sheetId="3" r:id="rId3"/>
+    <sheet name="BOP_3" sheetId="4" r:id="rId4"/>
+    <sheet name="BOP_4" sheetId="5" r:id="rId5"/>
+    <sheet name="BOP_5" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -399,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -432,7 +435,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>Package (MI)</v>
+        <v>BOP (MI)</v>
       </c>
       <c r="C2" t="str">
         <v>N/A</v>
@@ -444,7 +447,7 @@
         <v>FAILED</v>
       </c>
       <c r="F2" t="str">
-        <v>144.97</v>
+        <v>134.88</v>
       </c>
       <c r="G2" t="str">
         <v>MI</v>
@@ -455,27 +458,96 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>Package (PA)</v>
+        <v>BOP (WI)</v>
       </c>
       <c r="C3" t="str">
-        <v>3003179724</v>
+        <v>3003179758</v>
       </c>
       <c r="D3" t="str">
-        <v>N/A</v>
+        <v>1003052794</v>
       </c>
       <c r="E3" t="str">
-        <v>FAILED</v>
+        <v>PASSED</v>
       </c>
       <c r="F3" t="str">
-        <v>364.17</v>
+        <v>464.00</v>
       </c>
       <c r="G3" t="str">
+        <v>WI</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>BOP (DE)</v>
+      </c>
+      <c r="C4" t="str">
+        <v>3003179757</v>
+      </c>
+      <c r="D4" t="str">
+        <v>1003052797</v>
+      </c>
+      <c r="E4" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="F4" t="str">
+        <v>473.12</v>
+      </c>
+      <c r="G4" t="str">
+        <v>DE</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>BOP (PA)</v>
+      </c>
+      <c r="C5" t="str">
+        <v>3003179759</v>
+      </c>
+      <c r="D5" t="str">
+        <v>1003052795</v>
+      </c>
+      <c r="E5" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="F5" t="str">
+        <v>474.18</v>
+      </c>
+      <c r="G5" t="str">
         <v>PA</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>BOP (OH)</v>
+      </c>
+      <c r="C6" t="str">
+        <v>3003179760</v>
+      </c>
+      <c r="D6" t="str">
+        <v>1003052796</v>
+      </c>
+      <c r="E6" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="F6" t="str">
+        <v>468.78</v>
+      </c>
+      <c r="G6" t="str">
+        <v>OH</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -509,10 +581,10 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>78.94s</v>
+        <v>69.30s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-26T13:03:17.027Z</v>
+        <v>2025-12-26T14:54:21.518Z</v>
       </c>
     </row>
     <row r="3">
@@ -523,10 +595,10 @@
         <v>FAILED</v>
       </c>
       <c r="C3" t="str">
-        <v>66.03s</v>
+        <v>65.58s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-26T13:04:23.060Z</v>
+        <v>2025-12-26T14:55:27.106Z</v>
       </c>
     </row>
   </sheetData>
@@ -538,7 +610,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -565,29 +637,421 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>79.47s</v>
+        <v>69.29s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-26T13:03:17.498Z</v>
+        <v>2025-12-26T14:54:16.289Z</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Test Execution Failed</v>
+        <v>Building and Classification Added</v>
       </c>
       <c r="B3" t="str">
-        <v>FAILED</v>
+        <v>PASSED</v>
       </c>
       <c r="C3" t="str">
-        <v>284.70s</v>
+        <v>142.62s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-26T13:08:02.197Z</v>
+        <v>2025-12-26T14:56:38.914Z</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Quote Rated Successfully</v>
+      </c>
+      <c r="B4" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C4" t="str">
+        <v>22.45s</v>
+      </c>
+      <c r="D4" t="str">
+        <v>2025-12-26T14:57:01.369Z</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Submitting for Approval</v>
+      </c>
+      <c r="B5" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C5" t="str">
+        <v>33.98s</v>
+      </c>
+      <c r="D5" t="str">
+        <v>2025-12-26T14:57:35.356Z</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>UW Issues Approved in PolicyCenter</v>
+      </c>
+      <c r="B6" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C6" t="str">
+        <v>44.90s</v>
+      </c>
+      <c r="D6" t="str">
+        <v>2025-12-26T14:58:20.253Z</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Policy Issued Successfully</v>
+      </c>
+      <c r="B7" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C7" t="str">
+        <v>150.76s</v>
+      </c>
+      <c r="D7" t="str">
+        <v>2025-12-26T15:00:51.014Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Milestone</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Duration (s)</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Timestamp</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Account Created</v>
+      </c>
+      <c r="B2" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C2" t="str">
+        <v>71.25s</v>
+      </c>
+      <c r="D2" t="str">
+        <v>2025-12-26T14:54:15.823Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Building and Classification Added</v>
+      </c>
+      <c r="B3" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C3" t="str">
+        <v>150.96s</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2025-12-26T14:56:46.787Z</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Quote Rated Successfully</v>
+      </c>
+      <c r="B4" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C4" t="str">
+        <v>23.44s</v>
+      </c>
+      <c r="D4" t="str">
+        <v>2025-12-26T14:57:10.233Z</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Submitting for Approval</v>
+      </c>
+      <c r="B5" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C5" t="str">
+        <v>35.31s</v>
+      </c>
+      <c r="D5" t="str">
+        <v>2025-12-26T14:57:45.551Z</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>UW Issues Approved in PolicyCenter</v>
+      </c>
+      <c r="B6" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C6" t="str">
+        <v>41.13s</v>
+      </c>
+      <c r="D6" t="str">
+        <v>2025-12-26T14:58:26.685Z</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Policy Issued Successfully</v>
+      </c>
+      <c r="B7" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C7" t="str">
+        <v>151.03s</v>
+      </c>
+      <c r="D7" t="str">
+        <v>2025-12-26T15:00:57.717Z</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Milestone</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Duration (s)</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Timestamp</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Account Created</v>
+      </c>
+      <c r="B2" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C2" t="str">
+        <v>71.17s</v>
+      </c>
+      <c r="D2" t="str">
+        <v>2025-12-26T14:54:16.685Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Building and Classification Added</v>
+      </c>
+      <c r="B3" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C3" t="str">
+        <v>150.67s</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2025-12-26T14:56:47.355Z</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Quote Rated Successfully</v>
+      </c>
+      <c r="B4" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C4" t="str">
+        <v>24.13s</v>
+      </c>
+      <c r="D4" t="str">
+        <v>2025-12-26T14:57:11.486Z</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Submitting for Approval</v>
+      </c>
+      <c r="B5" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C5" t="str">
+        <v>34.10s</v>
+      </c>
+      <c r="D5" t="str">
+        <v>2025-12-26T14:57:45.584Z</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>UW Issues Approved in PolicyCenter</v>
+      </c>
+      <c r="B6" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C6" t="str">
+        <v>41.95s</v>
+      </c>
+      <c r="D6" t="str">
+        <v>2025-12-26T14:58:27.539Z</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Policy Issued Successfully</v>
+      </c>
+      <c r="B7" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C7" t="str">
+        <v>152.16s</v>
+      </c>
+      <c r="D7" t="str">
+        <v>2025-12-26T15:00:59.697Z</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Milestone</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Duration (s)</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Timestamp</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Account Created</v>
+      </c>
+      <c r="B2" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C2" t="str">
+        <v>69.89s</v>
+      </c>
+      <c r="D2" t="str">
+        <v>2025-12-26T14:54:21.586Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Building and Classification Added</v>
+      </c>
+      <c r="B3" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C3" t="str">
+        <v>140.51s</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2025-12-26T14:56:42.103Z</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Quote Rated Successfully</v>
+      </c>
+      <c r="B4" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C4" t="str">
+        <v>32.18s</v>
+      </c>
+      <c r="D4" t="str">
+        <v>2025-12-26T14:57:14.288Z</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Submitting for Approval</v>
+      </c>
+      <c r="B5" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C5" t="str">
+        <v>33.88s</v>
+      </c>
+      <c r="D5" t="str">
+        <v>2025-12-26T14:57:48.170Z</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>UW Issues Approved in PolicyCenter</v>
+      </c>
+      <c r="B6" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C6" t="str">
+        <v>40.41s</v>
+      </c>
+      <c r="D6" t="str">
+        <v>2025-12-26T14:58:28.587Z</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Policy Issued Successfully</v>
+      </c>
+      <c r="B7" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C7" t="str">
+        <v>151.91s</v>
+      </c>
+      <c r="D7" t="str">
+        <v>2025-12-26T15:01:00.497Z</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Enhance parallel runners: up to 3 jobs, 30s staggered start, improved status logic for BOP and Package
</commit_message>
<xml_diff>
--- a/WB_Test_Report_2025-12-26.xlsx
+++ b/WB_Test_Report_2025-12-26.xlsx
@@ -4,11 +4,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="BOP_1" sheetId="2" r:id="rId2"/>
-    <sheet name="BOP_2" sheetId="3" r:id="rId3"/>
-    <sheet name="BOP_3" sheetId="4" r:id="rId4"/>
-    <sheet name="BOP_4" sheetId="5" r:id="rId5"/>
-    <sheet name="BOP_5" sheetId="6" r:id="rId6"/>
+    <sheet name="Package_1" sheetId="2" r:id="rId2"/>
+    <sheet name="Package_2" sheetId="3" r:id="rId3"/>
+    <sheet name="Package_3" sheetId="4" r:id="rId4"/>
+    <sheet name="Package_4" sheetId="5" r:id="rId5"/>
+    <sheet name="Package_5" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -435,7 +435,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>BOP (MI)</v>
+        <v>Package (OH)</v>
       </c>
       <c r="C2" t="str">
         <v>N/A</v>
@@ -447,10 +447,10 @@
         <v>FAILED</v>
       </c>
       <c r="F2" t="str">
-        <v>134.88</v>
+        <v>200.98</v>
       </c>
       <c r="G2" t="str">
-        <v>MI</v>
+        <v>OH</v>
       </c>
     </row>
     <row r="3">
@@ -458,22 +458,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>BOP (WI)</v>
+        <v>Package (PA)</v>
       </c>
       <c r="C3" t="str">
-        <v>3003179758</v>
+        <v>3003179815</v>
       </c>
       <c r="D3" t="str">
-        <v>1003052794</v>
+        <v>N/A</v>
       </c>
       <c r="E3" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="F3" t="str">
-        <v>464.00</v>
+        <v>144.59</v>
       </c>
       <c r="G3" t="str">
-        <v>WI</v>
+        <v>PA</v>
       </c>
     </row>
     <row r="4">
@@ -481,22 +481,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>BOP (DE)</v>
+        <v>Package (MI)</v>
       </c>
       <c r="C4" t="str">
-        <v>3003179757</v>
+        <v>3003179443</v>
       </c>
       <c r="D4" t="str">
-        <v>1003052797</v>
+        <v>N/A</v>
       </c>
       <c r="E4" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="F4" t="str">
-        <v>473.12</v>
+        <v>135.88</v>
       </c>
       <c r="G4" t="str">
-        <v>DE</v>
+        <v>MI</v>
       </c>
     </row>
     <row r="5">
@@ -504,22 +504,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <v>BOP (PA)</v>
+        <v>Package (WI)</v>
       </c>
       <c r="C5" t="str">
-        <v>3003179759</v>
+        <v>3003179818</v>
       </c>
       <c r="D5" t="str">
-        <v>1003052795</v>
+        <v>1003052814</v>
       </c>
       <c r="E5" t="str">
         <v>PASSED</v>
       </c>
       <c r="F5" t="str">
-        <v>474.18</v>
+        <v>868.26</v>
       </c>
       <c r="G5" t="str">
-        <v>PA</v>
+        <v>WI</v>
       </c>
     </row>
     <row r="6">
@@ -527,22 +527,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="str">
-        <v>BOP (OH)</v>
+        <v>Package (DE)</v>
       </c>
       <c r="C6" t="str">
-        <v>3003179760</v>
+        <v>3003179825</v>
       </c>
       <c r="D6" t="str">
-        <v>1003052796</v>
+        <v>1003052816</v>
       </c>
       <c r="E6" t="str">
         <v>PASSED</v>
       </c>
       <c r="F6" t="str">
-        <v>468.78</v>
+        <v>819.88</v>
       </c>
       <c r="G6" t="str">
-        <v>OH</v>
+        <v>DE</v>
       </c>
     </row>
   </sheetData>
@@ -581,10 +581,10 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>69.30s</v>
+        <v>76.24s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-26T14:54:21.518Z</v>
+        <v>2025-12-26T21:04:29.011Z</v>
       </c>
     </row>
     <row r="3">
@@ -595,10 +595,10 @@
         <v>FAILED</v>
       </c>
       <c r="C3" t="str">
-        <v>65.58s</v>
+        <v>124.74s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-26T14:55:27.106Z</v>
+        <v>2025-12-26T21:06:33.750Z</v>
       </c>
     </row>
   </sheetData>
@@ -610,7 +610,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -637,92 +637,36 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>69.29s</v>
+        <v>72.39s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-26T14:54:16.289Z</v>
+        <v>2025-12-26T21:07:51.396Z</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Building and Classification Added</v>
+        <v>Test Execution Failed</v>
       </c>
       <c r="B3" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="C3" t="str">
-        <v>142.62s</v>
+        <v>72.20s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-26T14:56:38.914Z</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Quote Rated Successfully</v>
-      </c>
-      <c r="B4" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C4" t="str">
-        <v>22.45s</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2025-12-26T14:57:01.369Z</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Submitting for Approval</v>
-      </c>
-      <c r="B5" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C5" t="str">
-        <v>33.98s</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2025-12-26T14:57:35.356Z</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>UW Issues Approved in PolicyCenter</v>
-      </c>
-      <c r="B6" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C6" t="str">
-        <v>44.90s</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2025-12-26T14:58:20.253Z</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Policy Issued Successfully</v>
-      </c>
-      <c r="B7" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C7" t="str">
-        <v>150.76s</v>
-      </c>
-      <c r="D7" t="str">
-        <v>2025-12-26T15:00:51.014Z</v>
+        <v>2025-12-26T21:09:03.597Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -749,92 +693,36 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>71.25s</v>
+        <v>72.84s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-26T14:54:15.823Z</v>
+        <v>2025-12-26T21:10:22.626Z</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Building and Classification Added</v>
+        <v>Test Execution Failed</v>
       </c>
       <c r="B3" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="C3" t="str">
-        <v>150.96s</v>
+        <v>63.04s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-26T14:56:46.787Z</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Quote Rated Successfully</v>
-      </c>
-      <c r="B4" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C4" t="str">
-        <v>23.44s</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2025-12-26T14:57:10.233Z</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Submitting for Approval</v>
-      </c>
-      <c r="B5" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C5" t="str">
-        <v>35.31s</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2025-12-26T14:57:45.551Z</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>UW Issues Approved in PolicyCenter</v>
-      </c>
-      <c r="B6" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C6" t="str">
-        <v>41.13s</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2025-12-26T14:58:26.685Z</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Policy Issued Successfully</v>
-      </c>
-      <c r="B7" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C7" t="str">
-        <v>151.03s</v>
-      </c>
-      <c r="D7" t="str">
-        <v>2025-12-26T15:00:57.717Z</v>
+        <v>2025-12-26T21:11:25.669Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -861,92 +749,134 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>71.17s</v>
+        <v>69.44s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-26T14:54:16.685Z</v>
+        <v>2025-12-26T21:12:44.181Z</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Building and Classification Added</v>
+        <v>Commercial Property Package Completed</v>
       </c>
       <c r="B3" t="str">
         <v>PASSED</v>
       </c>
       <c r="C3" t="str">
-        <v>150.67s</v>
+        <v>309.51s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-26T14:56:47.355Z</v>
+        <v>2025-12-26T21:17:53.690Z</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Quote Rated Successfully</v>
+        <v>General Liability Completed</v>
       </c>
       <c r="B4" t="str">
         <v>PASSED</v>
       </c>
       <c r="C4" t="str">
-        <v>24.13s</v>
+        <v>96.64s</v>
       </c>
       <c r="D4" t="str">
-        <v>2025-12-26T14:57:11.486Z</v>
+        <v>2025-12-26T21:19:30.331Z</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Submitting for Approval</v>
+        <v>Inland Marine Completed</v>
       </c>
       <c r="B5" t="str">
         <v>PASSED</v>
       </c>
       <c r="C5" t="str">
-        <v>34.10s</v>
+        <v>37.91s</v>
       </c>
       <c r="D5" t="str">
-        <v>2025-12-26T14:57:45.584Z</v>
+        <v>2025-12-26T21:20:08.242Z</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>UW Issues Approved in PolicyCenter</v>
+        <v>Crime Completed</v>
       </c>
       <c r="B6" t="str">
         <v>PASSED</v>
       </c>
       <c r="C6" t="str">
-        <v>41.95s</v>
+        <v>23.20s</v>
       </c>
       <c r="D6" t="str">
-        <v>2025-12-26T14:58:27.539Z</v>
+        <v>2025-12-26T21:20:31.444Z</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
+        <v>Quote Rated Successfully</v>
+      </c>
+      <c r="B7" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C7" t="str">
+        <v>85.87s</v>
+      </c>
+      <c r="D7" t="str">
+        <v>2025-12-26T21:21:57.319Z</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Submitting for Approval</v>
+      </c>
+      <c r="B8" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C8" t="str">
+        <v>36.22s</v>
+      </c>
+      <c r="D8" t="str">
+        <v>2025-12-26T21:22:33.540Z</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>UW Issues Approved in PolicyCenter</v>
+      </c>
+      <c r="B9" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C9" t="str">
+        <v>55.68s</v>
+      </c>
+      <c r="D9" t="str">
+        <v>2025-12-26T21:23:29.221Z</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
         <v>Policy Issued Successfully</v>
       </c>
-      <c r="B7" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C7" t="str">
-        <v>152.16s</v>
-      </c>
-      <c r="D7" t="str">
-        <v>2025-12-26T15:00:59.697Z</v>
+      <c r="B10" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C10" t="str">
+        <v>153.79s</v>
+      </c>
+      <c r="D10" t="str">
+        <v>2025-12-26T21:26:03.013Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D10"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -973,85 +903,127 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>69.89s</v>
+        <v>72.92s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-26T14:54:21.586Z</v>
+        <v>2025-12-26T21:26:26.929Z</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Building and Classification Added</v>
+        <v>Commercial Property Package Completed</v>
       </c>
       <c r="B3" t="str">
         <v>PASSED</v>
       </c>
       <c r="C3" t="str">
-        <v>140.51s</v>
+        <v>285.73s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-26T14:56:42.103Z</v>
+        <v>2025-12-26T21:31:12.662Z</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Quote Rated Successfully</v>
+        <v>General Liability Completed</v>
       </c>
       <c r="B4" t="str">
         <v>PASSED</v>
       </c>
       <c r="C4" t="str">
-        <v>32.18s</v>
+        <v>89.43s</v>
       </c>
       <c r="D4" t="str">
-        <v>2025-12-26T14:57:14.288Z</v>
+        <v>2025-12-26T21:32:42.097Z</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Submitting for Approval</v>
+        <v>Inland Marine Completed</v>
       </c>
       <c r="B5" t="str">
         <v>PASSED</v>
       </c>
       <c r="C5" t="str">
-        <v>33.88s</v>
+        <v>38.24s</v>
       </c>
       <c r="D5" t="str">
-        <v>2025-12-26T14:57:48.170Z</v>
+        <v>2025-12-26T21:33:20.340Z</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>UW Issues Approved in PolicyCenter</v>
+        <v>Crime Completed</v>
       </c>
       <c r="B6" t="str">
         <v>PASSED</v>
       </c>
       <c r="C6" t="str">
-        <v>40.41s</v>
+        <v>23.83s</v>
       </c>
       <c r="D6" t="str">
-        <v>2025-12-26T14:58:28.587Z</v>
+        <v>2025-12-26T21:33:44.170Z</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
+        <v>Quote Rated Successfully</v>
+      </c>
+      <c r="B7" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C7" t="str">
+        <v>60.21s</v>
+      </c>
+      <c r="D7" t="str">
+        <v>2025-12-26T21:34:44.379Z</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Submitting for Approval</v>
+      </c>
+      <c r="B8" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C8" t="str">
+        <v>34.26s</v>
+      </c>
+      <c r="D8" t="str">
+        <v>2025-12-26T21:35:18.645Z</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>UW Issues Approved in PolicyCenter</v>
+      </c>
+      <c r="B9" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C9" t="str">
+        <v>63.03s</v>
+      </c>
+      <c r="D9" t="str">
+        <v>2025-12-26T21:36:21.674Z</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
         <v>Policy Issued Successfully</v>
       </c>
-      <c r="B7" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C7" t="str">
-        <v>151.91s</v>
-      </c>
-      <c r="D7" t="str">
-        <v>2025-12-26T15:01:00.497Z</v>
+      <c r="B10" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C10" t="str">
+        <v>152.23s</v>
+      </c>
+      <c r="D10" t="str">
+        <v>2025-12-26T21:38:53.907Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>